<commit_message>
DOSINZAGE2-307: Removed test instance without corresponding DICOM files
</commit_message>
<xml_diff>
--- a/test/testdata/Testdata_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
+++ b/test/testdata/Testdata_MedMij_Beeldbeschikbaarheid_1.0.0-beta.1.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-Images/test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/luudslagter/Documents/git/MedMij-R4-ImageAvailability/test/testdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBF79765-7FE6-D443-B250-508E2F0799ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D09676FC-43D5-A745-A6C2-7055E378AAED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29560" yWindow="660" windowWidth="34140" windowHeight="27980" xr2:uid="{1650A346-D655-9F40-A836-70310FE71EFF}"/>
+    <workbookView xWindow="29540" yWindow="660" windowWidth="68480" windowHeight="27980" xr2:uid="{1650A346-D655-9F40-A836-70310FE71EFF}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="263" uniqueCount="127">
   <si>
     <t>Testcase</t>
   </si>
@@ -317,9 +317,6 @@
     <t>5.3</t>
   </si>
   <si>
-    <t>5.4</t>
-  </si>
-  <si>
     <t>999990019</t>
   </si>
   <si>
@@ -347,9 +344,6 @@
     <t>01.015 (Huisarts)</t>
   </si>
   <si>
-    <t>113091000 - MRI</t>
-  </si>
-  <si>
     <t>77477000 - CT</t>
   </si>
   <si>
@@ -362,9 +356,6 @@
     <t>V6 Algemeen ziekenhuis</t>
   </si>
   <si>
-    <t>b7e5d9e2-9e5f-4df6-bc0f-9f98b6d4c705</t>
-  </si>
-  <si>
     <t>23-05-2024 - 12:00</t>
   </si>
   <si>
@@ -378,18 +369,6 @@
   </si>
   <si>
     <t>03-03-2020 - 12:00</t>
-  </si>
-  <si>
-    <t>07-08-2024 - 11:57</t>
-  </si>
-  <si>
-    <t>MedMij PGO test MR</t>
-  </si>
-  <si>
-    <t>EXT-14115</t>
-  </si>
-  <si>
-    <t>2.16.840.1.114493.1.4.270.3.20240807115710430</t>
   </si>
   <si>
     <t>a013c0cf-d4f9-4bc5-aa76-ac41347454bd</t>
@@ -927,10 +906,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F9EBAD-47C5-D644-9667-952271EB079B}">
-  <dimension ref="A1:AA12"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -976,7 +955,7 @@
         <v>43</v>
       </c>
       <c r="D1" s="12" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="E1" s="12" t="s">
         <v>54</v>
@@ -1089,7 +1068,7 @@
         <v>5</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>6</v>
@@ -1110,7 +1089,7 @@
         <v>70</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="V2" s="4" t="s">
         <v>83</v>
@@ -1119,7 +1098,7 @@
         <v>71</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>84</v>
@@ -1193,7 +1172,7 @@
         <v>72</v>
       </c>
       <c r="U3" s="7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="V3" s="7" t="s">
         <v>85</v>
@@ -1285,7 +1264,7 @@
         <v>73</v>
       </c>
       <c r="X4" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="Y4" s="7" t="s">
         <v>85</v>
@@ -1359,7 +1338,7 @@
         <v>74</v>
       </c>
       <c r="U5" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="V5" s="7" t="s">
         <v>85</v>
@@ -1368,7 +1347,7 @@
         <v>75</v>
       </c>
       <c r="X5" s="7" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="Y5" s="7" t="s">
         <v>85</v>
@@ -1442,7 +1421,7 @@
         <v>76</v>
       </c>
       <c r="U6" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="V6" s="7" t="s">
         <v>86</v>
@@ -1451,7 +1430,7 @@
         <v>77</v>
       </c>
       <c r="X6" s="7" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="Y6" s="7" t="s">
         <v>86</v>
@@ -1504,7 +1483,7 @@
         <v>5</v>
       </c>
       <c r="N7" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>6</v>
@@ -1525,7 +1504,7 @@
         <v>78</v>
       </c>
       <c r="U7" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="V7" s="4" t="s">
         <v>87</v>
@@ -1634,19 +1613,19 @@
         <v>90</v>
       </c>
       <c r="B9" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="G9" s="4">
         <v>18296</v>
@@ -1655,61 +1634,61 @@
         <v>14</v>
       </c>
       <c r="I9" s="4">
-        <v>45511</v>
+        <v>45526</v>
       </c>
       <c r="J9" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="K9" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="L9" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M9" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="L9" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="M9" s="3" t="s">
+      <c r="N9" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S9" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="N9" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="O9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S9" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="T9" s="3" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="U9" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="V9" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="W9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="X9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Y9" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Z9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="AA9" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="V9" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="W9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="X9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y9" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z9" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="AA9" s="3" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="17" x14ac:dyDescent="0.2">
@@ -1717,19 +1696,19 @@
         <v>91</v>
       </c>
       <c r="B10" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D10" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="G10" s="4">
         <v>18296</v>
@@ -1738,43 +1717,43 @@
         <v>14</v>
       </c>
       <c r="I10" s="4">
-        <v>45526</v>
+        <v>45674</v>
       </c>
       <c r="J10" s="15" t="s">
+        <v>102</v>
+      </c>
+      <c r="K10" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="L10" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K10" s="20" t="s">
+      <c r="M10" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="M10" s="3" t="s">
+      <c r="N10" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="O10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="R10" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="S10" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="N10" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R10" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S10" s="3" t="s">
-        <v>101</v>
-      </c>
       <c r="T10" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="U10" s="4" t="s">
         <v>118</v>
-      </c>
-      <c r="U10" s="4" t="s">
-        <v>123</v>
       </c>
       <c r="V10" s="4" t="s">
         <v>119</v>
@@ -1800,19 +1779,19 @@
         <v>92</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>6</v>
       </c>
       <c r="D11" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="G11" s="4">
         <v>18296</v>
@@ -1824,19 +1803,19 @@
         <v>45674</v>
       </c>
       <c r="J11" s="15" t="s">
+        <v>103</v>
+      </c>
+      <c r="K11" s="20" t="s">
+        <v>98</v>
+      </c>
+      <c r="L11" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="K11" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="L11" s="3" t="s">
-        <v>106</v>
-      </c>
       <c r="M11" s="3" t="s">
-        <v>100</v>
+        <v>6</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>6</v>
@@ -1857,108 +1836,25 @@
         <v>122</v>
       </c>
       <c r="U11" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="V11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="W11" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="X11" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="V11" s="4" t="s">
+      <c r="Y11" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>5003249215</v>
+      </c>
+      <c r="AA11" s="3" t="s">
         <v>126</v>
-      </c>
-      <c r="W11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="X11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Y11" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Z11" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="AA11" s="3" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="17" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>93</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="G12" s="4">
-        <v>18296</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="I12" s="4">
-        <v>45674</v>
-      </c>
-      <c r="J12" s="15" t="s">
-        <v>105</v>
-      </c>
-      <c r="K12" s="20" t="s">
-        <v>99</v>
-      </c>
-      <c r="L12" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="M12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="N12" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="O12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="P12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="Q12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="R12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="S12" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="T12" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="U12" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="V12" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="W12" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="X12" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="Y12" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="Z12" s="3">
-        <v>5003249215</v>
-      </c>
-      <c r="AA12" s="3" t="s">
-        <v>133</v>
       </c>
     </row>
   </sheetData>
@@ -1966,32 +1862,12 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
   <ignoredErrors>
-    <ignoredError sqref="K9:K11 B9:B11 K12 B12" numberStoredAsText="1"/>
+    <ignoredError sqref="K9:K10 B9:B10 K11 B11" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100597771DCE5E0DD409E6796B5544574D3" ma:contentTypeVersion="14" ma:contentTypeDescription="Een nieuw document maken." ma:contentTypeScope="" ma:versionID="1f155c61874143f60c84865cea76726f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xmlns:ns3="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7515b2bcca035c7557d524d6ba7a724c" ns2:_="" ns3:_="">
     <xsd:import namespace="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
@@ -2220,32 +2096,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{381658C6-125F-4228-83B4-050ACEF74B3B}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D2DF77-57FD-466E-B6E2-147D6ED80D92}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="7be6589a-2b09-4451-a4d9-5c4f513f6c62" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A85AB6D9-DC84-473F-93E0-175F4EA5C2B2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2264,6 +2135,31 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B2D2DF77-57FD-466E-B6E2-147D6ED80D92}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{381658C6-125F-4228-83B4-050ACEF74B3B}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="abb14ec8-0b0a-4bff-b394-a2c6c2dbafc7"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="7be6589a-2b09-4451-a4d9-5c4f513f6c62"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{72c2d0db-a1e3-4b16-91a1-67936a5cf3bf}" enabled="0" method="" siteId="{72c2d0db-a1e3-4b16-91a1-67936a5cf3bf}" removed="1"/>

</xml_diff>